<commit_message>
Report 报表 ----  Node 静态变量
</commit_message>
<xml_diff>
--- a/src/test/resources/Locator.xlsx
+++ b/src/test/resources/Locator.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\AppTest\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IdeaProJect\AppTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7776" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WelcomeAty" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -163,11 +163,39 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>首页Tab</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>水产Tab</t>
+    <t>android.support.v7.app.ActionBar$Tab</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>className</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.android.benlailife.activity:id/tvCenterLogin</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码登录</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.android.benlailife.activity:id/rb_login_password</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码登录btn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.android.benlailife.activity:id/btn_password_login</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.android.benlailife.activity:id/tvCenterSetting</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -175,46 +203,18 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>android.support.v7.app.ActionBar$Tab</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>className</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.android.benlailife.activity:id/tvCenterLogin</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码登录</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.android.benlailife.activity:id/rb_login_password</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>密码登录btn</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.android.benlailife.activity:id/btn_password_login</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>设置</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>com.android.benlailife.activity:id/tvCenterSetting</t>
+    <t>Tab</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.android.benlailife.activity:id/img_tab_center</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -616,11 +616,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -632,18 +632,18 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A4" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="65.625" customWidth="1"/>
-    <col min="3" max="3" width="21.125" customWidth="1"/>
-    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -671,7 +671,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -685,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -713,7 +713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -727,7 +727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -741,7 +741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -755,7 +755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -769,7 +769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -783,7 +783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>34</v>
       </c>
@@ -811,26 +811,26 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="C13" s="4">
         <v>3</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C14" s="4">
         <v>3</v>
@@ -839,61 +839,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -908,18 +908,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.5" customWidth="1"/>
+    <col min="2" max="2" width="58.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -933,12 +933,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4">
         <v>6</v>
@@ -947,18 +947,88 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -975,14 +1045,14 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="58.25" customWidth="1"/>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -996,12 +1066,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4">
         <v>3</v>
@@ -1010,7 +1080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1024,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1038,12 +1108,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4">
         <v>3</v>

</xml_diff>